<commit_message>
updated convert excel file to datatable
</commit_message>
<xml_diff>
--- a/SF.Utils.Tests/files/workbook files/file_example_XLSX_50.xlsx
+++ b/SF.Utils.Tests/files/workbook files/file_example_XLSX_50.xlsx
@@ -5,361 +5,366 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="205" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="115">
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Dulce</t>
-  </si>
-  <si>
-    <t>Abril</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>15/10/2017</t>
-  </si>
-  <si>
-    <t>Mara</t>
-  </si>
-  <si>
-    <t>Hashimoto</t>
-  </si>
-  <si>
-    <t>Great Britain</t>
-  </si>
-  <si>
-    <t>16/08/2016</t>
-  </si>
-  <si>
-    <t>Philip</t>
-  </si>
-  <si>
-    <t>Gent</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>21/05/2015</t>
-  </si>
-  <si>
-    <t>Kathleen</t>
-  </si>
-  <si>
-    <t>Hanner</t>
-  </si>
-  <si>
-    <t>Nereida</t>
-  </si>
-  <si>
-    <t>Magwood</t>
-  </si>
-  <si>
-    <t>Gaston</t>
-  </si>
-  <si>
-    <t>Brumm</t>
-  </si>
-  <si>
-    <t>Etta</t>
-  </si>
-  <si>
-    <t>Hurn</t>
-  </si>
-  <si>
-    <t>Earlean</t>
-  </si>
-  <si>
-    <t>Melgar</t>
-  </si>
-  <si>
-    <t>Vincenza</t>
-  </si>
-  <si>
-    <t>Weiland</t>
-  </si>
-  <si>
-    <t>Fallon</t>
-  </si>
-  <si>
-    <t>Winward</t>
-  </si>
-  <si>
-    <t>Arcelia</t>
-  </si>
-  <si>
-    <t>Bouska</t>
-  </si>
-  <si>
-    <t>Franklyn</t>
-  </si>
-  <si>
-    <t>Unknow</t>
-  </si>
-  <si>
-    <t>Sherron</t>
-  </si>
-  <si>
-    <t>Ascencio</t>
-  </si>
-  <si>
-    <t>Marcel</t>
-  </si>
-  <si>
-    <t>Zabriskie</t>
-  </si>
-  <si>
-    <t>Kina</t>
-  </si>
-  <si>
-    <t>Hazelton</t>
-  </si>
-  <si>
-    <t>Shavonne</t>
-  </si>
-  <si>
-    <t>Pia</t>
-  </si>
-  <si>
-    <t>Shavon</t>
-  </si>
-  <si>
-    <t>Benito</t>
-  </si>
-  <si>
-    <t>Lauralee</t>
-  </si>
-  <si>
-    <t>Perrine</t>
-  </si>
-  <si>
-    <t>Loreta</t>
-  </si>
-  <si>
-    <t>Curren</t>
-  </si>
-  <si>
-    <t>Teresa</t>
-  </si>
-  <si>
-    <t>Strawn</t>
-  </si>
-  <si>
-    <t>Belinda</t>
-  </si>
-  <si>
-    <t>Partain</t>
-  </si>
-  <si>
-    <t>Holly</t>
-  </si>
-  <si>
-    <t>Eudy</t>
-  </si>
-  <si>
-    <t>Many</t>
-  </si>
-  <si>
-    <t>Cuccia</t>
-  </si>
-  <si>
-    <t>Libbie</t>
-  </si>
-  <si>
-    <t>Dalby</t>
-  </si>
-  <si>
-    <t>Lester</t>
-  </si>
-  <si>
-    <t>Prothro</t>
-  </si>
-  <si>
-    <t>Marvel</t>
-  </si>
-  <si>
-    <t>Hail</t>
-  </si>
-  <si>
-    <t>Angelyn</t>
-  </si>
-  <si>
-    <t>Vong</t>
-  </si>
-  <si>
-    <t>Francesca</t>
-  </si>
-  <si>
-    <t>Beaudreau</t>
-  </si>
-  <si>
-    <t>Garth</t>
-  </si>
-  <si>
-    <t>Gangi</t>
-  </si>
-  <si>
-    <t>Carla</t>
-  </si>
-  <si>
-    <t>Trumbull</t>
-  </si>
-  <si>
-    <t>Veta</t>
-  </si>
-  <si>
-    <t>Muntz</t>
-  </si>
-  <si>
-    <t>Stasia</t>
-  </si>
-  <si>
-    <t>Becker</t>
-  </si>
-  <si>
-    <t>Jona</t>
-  </si>
-  <si>
-    <t>Grindle</t>
-  </si>
-  <si>
-    <t>Judie</t>
-  </si>
-  <si>
-    <t>Claywell</t>
-  </si>
-  <si>
-    <t>Dewitt</t>
-  </si>
-  <si>
-    <t>Borger</t>
-  </si>
-  <si>
-    <t>Nena</t>
-  </si>
-  <si>
-    <t>Hacker</t>
-  </si>
-  <si>
-    <t>Kelsie</t>
-  </si>
-  <si>
-    <t>Wachtel</t>
-  </si>
-  <si>
-    <t>Sau</t>
-  </si>
-  <si>
-    <t>Pfau</t>
-  </si>
-  <si>
-    <t>Shanice</t>
-  </si>
-  <si>
-    <t>Mccrystal</t>
-  </si>
-  <si>
-    <t>Chase</t>
-  </si>
-  <si>
-    <t>Karner</t>
-  </si>
-  <si>
-    <t>Tommie</t>
-  </si>
-  <si>
-    <t>Underdahl</t>
-  </si>
-  <si>
-    <t>Dorcas</t>
-  </si>
-  <si>
-    <t>Darity</t>
-  </si>
-  <si>
-    <t>Angel</t>
-  </si>
-  <si>
-    <t>Sanor</t>
-  </si>
-  <si>
-    <t>Willodean</t>
-  </si>
-  <si>
-    <t>Harn</t>
-  </si>
-  <si>
-    <t>Weston</t>
-  </si>
-  <si>
-    <t>Martina</t>
-  </si>
-  <si>
-    <t>Roma</t>
-  </si>
-  <si>
-    <t>Lafollette</t>
-  </si>
-  <si>
-    <t>Felisa</t>
-  </si>
-  <si>
-    <t>Cail</t>
-  </si>
-  <si>
-    <t>Demetria</t>
-  </si>
-  <si>
-    <t>Abbey</t>
-  </si>
-  <si>
-    <t>Jeromy</t>
-  </si>
-  <si>
-    <t>Danz</t>
-  </si>
-  <si>
-    <t>Rasheeda</t>
-  </si>
-  <si>
-    <t>Alkire</t>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dulce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abril</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/10/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hashimoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Britain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/08/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/05/2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kathleen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hanner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nereida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magwood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brumm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hurn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earlean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melgar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vincenza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weiland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fallon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arcelia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franklyn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sherron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ascencio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zabriskie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazelton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shavonne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shavon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lauralee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perrine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loreta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belinda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eudy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuccia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libbie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prothro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marvel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angelyn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Francesca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaudreau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gangi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trumbull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muntz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stasia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Becker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grindle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claywell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dewitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Borger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kelsie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wachtel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shanice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mccrystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Underdahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorcas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willodean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lafollette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demetria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abbey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeromy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rasheeda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alkire</t>
   </si>
 </sst>
 </file>
@@ -367,7 +372,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="5">
@@ -375,6 +380,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -396,6 +402,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -459,12 +466,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -476,13 +483,13 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K46" activeCellId="0" sqref="K46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,7 +1821,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>